<commit_message>
test: add min & max test cases in Table cypress tests
</commit_message>
<xml_diff>
--- a/cypress/fixtures/customers_invalid.xlsx
+++ b/cypress/fixtures/customers_invalid.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="18">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t xml:space="preserve">bad_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/01/1899</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/01/2999</t>
   </si>
 </sst>
 </file>
@@ -83,6 +89,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -164,25 +171,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -335,7 +341,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>15</v>
+        <v>-1</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>9</v>
@@ -344,9 +350,49 @@
         <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>999</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>99.9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F11" s="0" t="n">
         <v>1.7</v>
       </c>
     </row>

</xml_diff>